<commit_message>
Updating a product's price will not affect original price of product shown in order history
</commit_message>
<xml_diff>
--- a/flask_project/data/awae_order2_item.xlsx
+++ b/flask_project/data/awae_order2_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HDD documents\University\comp3900\capstone-project-3900-h10a-awae\flask_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6EFE4A-E0D9-459A-A048-7FCCFCD42981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953A0C25-D0D3-4786-96C3-F16722A47FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0BAE7C70-C35C-42C5-96B4-0F314623E3BF}"/>
+    <workbookView xWindow="1476" yWindow="4836" windowWidth="18000" windowHeight="10776" xr2:uid="{0BAE7C70-C35C-42C5-96B4-0F314623E3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>order2_id</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804A472C-1C69-4F20-B1C5-54775BD8D03D}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,7 +409,7 @@
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +419,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,8 +433,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -438,8 +447,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -449,8 +461,11 @@
       <c r="C4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -460,8 +475,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -471,8 +489,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -482,8 +503,11 @@
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -493,8 +517,11 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -504,8 +531,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -515,8 +545,11 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -526,8 +559,11 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -536,6 +572,9 @@
       </c>
       <c r="C12">
         <v>2</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>